<commit_message>
Update to version v6.0.0
</commit_message>
<xml_diff>
--- a/.nightswatch/functional/files/import-fail.xlsx
+++ b/.nightswatch/functional/files/import-fail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msjangid/Desktop/myData/workspaces/nightswatch/src/NightsWatchSolutions/source/solutions-nightswatch-tests/qnabot-on-aws/regression-tests/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikemlin/f-team/awsaiml/src/Aws-ai-qna-bot/.nightswatch/functional/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10E2B80-173F-3447-B7BC-B89A407CEA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AEBAAB-89C8-F646-BCDA-08A9D565779C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{65063F85-4105-8F42-BAD0-641D55AA808E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{65063F85-4105-8F42-BAD0-641D55AA808E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>qid</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>enabletranslation2</t>
+  </si>
+  <si>
+    <t>No Spaces Warning</t>
   </si>
 </sst>
 </file>
@@ -513,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654EBFE9-4F2B-8349-985B-01DDB193FC33}">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,11 +720,53 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5" spans="1:27" ht="153" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{E35B1DD5-E194-D643-8879-83EB60A9A686}"/>
     <hyperlink ref="I3" r:id="rId2" xr:uid="{37D6FE7E-D8C0-8743-AF73-A5D36AE489F3}"/>
     <hyperlink ref="I4" r:id="rId3" xr:uid="{2BE65CD2-3570-E64D-A236-0E7589AD4093}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{51B3526F-BEA3-8645-9B36-ADCF99A9809B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to version v7.0.0
</commit_message>
<xml_diff>
--- a/.nightswatch/functional/files/import-fail.xlsx
+++ b/.nightswatch/functional/files/import-fail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikemlin/f-team/awsaiml/src/Aws-ai-qna-bot/.nightswatch/functional/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AEBAAB-89C8-F646-BCDA-08A9D565779C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84721ED-5141-A649-9B20-0F8C21303EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{65063F85-4105-8F42-BAD0-641D55AA808E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17660" xr2:uid="{65063F85-4105-8F42-BAD0-641D55AA808E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>qid</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>No Spaces Warning</t>
+  </si>
+  <si>
+    <t>QuestionCharLimitWarning</t>
+  </si>
+  <si>
+    <t>What will happen if I try to import a .json and/or excel (.xlsx) file containing a question/utterance with over 140 characters like this one?</t>
+  </si>
+  <si>
+    <t>What will happen if I try to import a .json and/or excel (.xlsx) file containing a question/utterance with over 140 characters like this one??</t>
+  </si>
+  <si>
+    <t>Questions/Utterances with over 140 Characters cannot be imported</t>
   </si>
 </sst>
 </file>
@@ -516,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654EBFE9-4F2B-8349-985B-01DDB193FC33}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,6 +773,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{E35B1DD5-E194-D643-8879-83EB60A9A686}"/>

</xml_diff>